<commit_message>
headerRows é propriedade do dialect e não do excel
</commit_message>
<xml_diff>
--- a/20230629T110916/1501.xlsx
+++ b/20230629T110916/1501.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjunior/Projects/splor/datapackage-reprex/20230629T110916/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE5C5B4-9EB5-0547-9617-9B7B799BC621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FAD913B-8CE9-D74A-9770-AED47B22ECF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{D88D13EC-1F5E-0B45-94A7-00BCFE4064F3}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'BASE OBZ'!$A$2:$D$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'BASE OBZ'!$A$2:$C$2</definedName>
     <definedName name="P026FUNED">'[1]AÇÕES E PROGRAMAS'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -63,30 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{7326088D-84D5-FB48-B4EB-21A255CDD7C3}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">AÇÃO VINCULADA AO PPAG
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>PARA INCLUIR UMA AÇÃO NOVA BASTA INSERIR UMA NOVA LINHA NA PLANILHA E FAZER O PREENCHIMENTO.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{20EEE3C7-BD76-AE4F-BD81-AA994DBBEDE3}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{20EEE3C7-BD76-AE4F-BD81-AA994DBBEDE3}">
       <text>
         <r>
           <rPr>
@@ -116,10 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
-  <si>
-    <t>INDICE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>PROJETO ORÇAMENTO BASE-ZERO</t>
   </si>
@@ -130,9 +104,6 @@
     <t>PROGRAMA</t>
   </si>
   <si>
-    <t>AÇÃO</t>
-  </si>
-  <si>
     <t>ELEMENTO</t>
   </si>
   <si>
@@ -140,9 +111,6 @@
   </si>
   <si>
     <t>060 - FORMACAO CULTURAL</t>
-  </si>
-  <si>
-    <t>1029 - ATIVIDADES DE ENSINO, FORMACAO E QUALIFICACAO PROFISSIONAL E TECNICA EM CULTURA E PATRIMONIO</t>
   </si>
   <si>
     <t>14 - DIÁRIAS - CIVIL</t>
@@ -158,27 +126,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,14 +163,8 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,12 +174,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -290,56 +229,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -708,7 +641,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
@@ -723,108 +656,85 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8278AE-E05E-BA44-A028-A76C8DCDD823}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="29.83203125" style="10" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="10"/>
+    <col min="1" max="1" width="32.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11"/>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
+    <row r="3" spans="1:3" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="4" spans="1:3" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="9" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+    <row r="6" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Favor selecionar uma opção disponível na lista. " sqref="A3:A5" xr:uid="{7247AD7B-A21A-C147-8389-821014091846}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Favor selecionar uma opção disponível na lista. Nela aparecem somente os programas vinculados à UO escolhida na coluna A. " sqref="B3:B6" xr:uid="{6CE5448F-E7E4-CE4A-8D95-0077650676A3}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Favor selecionar uma opção disponível na lista. Nela aparecem somente os ações vinculadas ao programa escolhido na coluna F. " sqref="C3:C6" xr:uid="{BA60A651-4A34-444C-A7E8-285894471232}">
-      <formula1>INDIRECT(#REF!)</formula1>
-    </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B1" location="INDICE!A1" display="INDICE" xr:uid="{FDABAA79-1201-3740-8C93-64E8C2270277}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>